<commit_message>
Task_BM16 |  Export PDF
</commit_message>
<xml_diff>
--- a/Data_Product/App_Data/template_QTGNGL.xlsx
+++ b/Data_Product/App_Data/template_QTGNGL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA_PR\Data_Product\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29FDF88A-DBA2-4E41-A86C-33A662C92982}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D954B3A9-830A-4EFC-85D3-98C5A512F63F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{B537A817-926E-4385-A812-CDE5F844F19A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">            TỔNG HỢP BẢNG DỮ LIỆU VỀ GANG LỎNG - GANG THỎI</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>DUC2</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
   </si>
 </sst>
 </file>
@@ -262,48 +265,48 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9504182-C7E2-4B49-8D1C-A3EC2355CE20}">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,102 +684,105 @@
     <col min="11" max="13" width="13.7109375" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" customWidth="1"/>
     <col min="15" max="16" width="11.5703125" customWidth="1"/>
-    <col min="17" max="17" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+    <row r="1" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+    <row r="2" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
-    <row r="4" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H4" s="2" t="s">
+    <row r="4" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
     </row>
-    <row r="7" spans="1:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:25" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K7" s="13" t="s">
@@ -785,64 +791,79 @@
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="P7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="13" t="s">
+      <c r="Q7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="4" t="s">
+    <row r="8" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="13"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="13"/>
     </row>
-    <row r="9" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
+    <row r="9" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A5:T5"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
@@ -850,15 +871,6 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A5:S5"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Task_BM16 | Update tool auto
</commit_message>
<xml_diff>
--- a/Data_Product/App_Data/template_QTGNGL.xlsx
+++ b/Data_Product/App_Data/template_QTGNGL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA_PR\Data_Product\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D954B3A9-830A-4EFC-85D3-98C5A512F63F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CC7B45-443A-4418-8D7E-967FB32CF92D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{B537A817-926E-4385-A812-CDE5F844F19A}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t xml:space="preserve">            TỔNG HỢP BẢNG DỮ LIỆU VỀ GANG LỎNG - GANG THỎI</t>
   </si>
   <si>
-    <t>Từ ngày:.... đến ngày:....... - Bộ phận: .........</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Ngày luyện :……………….. - Ca :………. - Kíp :……. - Lò cao :………..</t>
   </si>
 </sst>
 </file>
@@ -271,40 +271,40 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -668,7 +668,7 @@
   <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="A5" sqref="A5:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,26 +689,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="4" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H4" s="1" t="s">
@@ -731,106 +731,106 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
+      <c r="A5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
     </row>
     <row r="7" spans="1:25" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="D7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="P7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="14" t="s">
+      <c r="Q7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="P7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q7" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="R7" s="13" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="6"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="16"/>
       <c r="K8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="M8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="13"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:25" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -854,6 +854,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="A5:T5"/>
     <mergeCell ref="K7:N7"/>
@@ -870,7 +871,6 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>